<commit_message>
add halaman, fix random, p2-52
</commit_message>
<xml_diff>
--- a/data kalimat durusul lughoh 2.xlsx
+++ b/data kalimat durusul lughoh 2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\trial\barab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\trial\githurtfmplizio\rtfmpliz.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{120C85C5-2AB4-40E4-A2FB-B2A7841E3D04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80ABE215-9868-466E-B7FA-E93772C49281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{998D3561-EEEE-4E4F-800B-72A3D3D90E3C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>id</t>
   </si>
@@ -90,6 +90,144 @@
   </si>
   <si>
     <t>ya, aku sudah pergi</t>
+  </si>
+  <si>
+    <t>dimana kalian (lk) pergi setelah pelajaran wahai anak2 ku ?</t>
+  </si>
+  <si>
+    <t>kami pergi ke tempat bermain</t>
+  </si>
+  <si>
+    <t>apakah sepak bola kalian bermain atau bola basket ?</t>
+  </si>
+  <si>
+    <t>hari ini kami bermain sepak bola. Kami bermain bola baske pekan kemarin</t>
+  </si>
+  <si>
+    <t>tidakkah kalian pergi ke perpustakaan hari ini ?</t>
+  </si>
+  <si>
+    <t>benar, kami telah pergi</t>
+  </si>
+  <si>
+    <t>apa (yang) kalian baca disana ?</t>
+  </si>
+  <si>
+    <t>kami telah membaca koran</t>
+  </si>
+  <si>
+    <t>apakah kalian mendegar berita ? Kabar dari radio hari ini ?</t>
+  </si>
+  <si>
+    <t>dari mana radio yang kalian dengar ?</t>
+  </si>
+  <si>
+    <t>kami mendengar dari 3 radio: dari radio riyadh, dan radio kairo, dan radio london</t>
+  </si>
+  <si>
+    <t>aku telah mendengar bahwasannya bilal sakit dan bahwasanya dia di rumah sakit. Apakah benar ini ?</t>
+  </si>
+  <si>
+    <t>ya, kami mendengar nya</t>
+  </si>
+  <si>
+    <t>ya, ini benar, semoga Allah menyembuhkannya</t>
+  </si>
+  <si>
+    <t>hal</t>
+  </si>
+  <si>
+    <t>aamiin, kapan dia (lk) masuk rumah sakit ?</t>
+  </si>
+  <si>
+    <t>dia (lk) masuk 3 hari yang lalu / sebelumnya (sebelum 3 hari)</t>
+  </si>
+  <si>
+    <t>dimana kitab (tersebut) yang memiliki sampul merah yang (dulu) didalam kamarku ? Apakah kalian )lk melihatnya ?</t>
+  </si>
+  <si>
+    <t>saya mengambilnya semalam dan saya membaca separuh</t>
+  </si>
+  <si>
+    <t>dan dimana majalah (tersebut) yang (dulu) dibawah kitab (tersebut) ini ?</t>
+  </si>
+  <si>
+    <t>apakah ini dia ?</t>
+  </si>
+  <si>
+    <t>tidak, majalah (tersebut) memiliki sampul kuning</t>
+  </si>
+  <si>
+    <t>dia bersamaku, aku mengambilnya hari ini</t>
+  </si>
+  <si>
+    <t>bell telah berbunyi maka marwan berdiri dan sedang membuka pintu (tersebut) dan saudara (pr) nya (sedang ) masuk</t>
+  </si>
+  <si>
+    <t>assalaamu 'alaikum warohmatullohi wabarokaatuh</t>
+  </si>
+  <si>
+    <t>wa 'alaikum salaam warohmatullohi wabarokaatuh</t>
+  </si>
+  <si>
+    <t>dimana kalian (pr) (telah) pergi wahai anak-anaku (pr)</t>
+  </si>
+  <si>
+    <t>kami pergi untuk mengunjungi kepala sekolah (pr, tersebut)</t>
+  </si>
+  <si>
+    <t>apakah kalian (pr) berjalan atau kalian (pr) pergi dengan mobil ?</t>
+  </si>
+  <si>
+    <t>kami berjalan dikarenakan rumahnya (pr) dekan dari sekolah kami. Dia diantara masjid dan sekolah</t>
+  </si>
+  <si>
+    <t>apakah kalian (pr) menjumpainya (pr) di dalam rumah (tersebut)</t>
+  </si>
+  <si>
+    <t>ya, kami menjumpainya (pr). Kami duduk bersamanya (pr) 1/3 jam dan kami keluar dari rumahnya (pr) di jam (ke) 5</t>
+  </si>
+  <si>
+    <t>aku meletakkannya dibawah tangga (tsb) pagi (subuh) ini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apakah kalian (pr) melihat sapu (tsb) wahai anak-anak (pr) ? Aku mencari nya berkali-kali dan aku tidak menemukannya </t>
+  </si>
+  <si>
+    <t>wahai ibuku, apakah didalam kulkas ada air dingin ? Kamu haus</t>
+  </si>
+  <si>
+    <t>berbahagialah, didalamnya ada air dingin, dan jus jeruk</t>
+  </si>
+  <si>
+    <t>jawablah dari pertanyaan-pertanyaan berikut</t>
+  </si>
+  <si>
+    <t>dimana anak-anak (lk) setelah pelajaran ?</t>
+  </si>
+  <si>
+    <t>kapan mereka (lk) (telah) membaca didalam perpustakaan ?</t>
+  </si>
+  <si>
+    <t>dari radio mana mereka (lk) mendengar kabar ?</t>
+  </si>
+  <si>
+    <t>siapa yang telah mengambil kitab (tsb)</t>
+  </si>
+  <si>
+    <t>siapa yang (telah) mengambil majalah (tsb) ?</t>
+  </si>
+  <si>
+    <t>dimana anak-anak (pr) (telah) pergi ?</t>
+  </si>
+  <si>
+    <t>berapa menit mereka (pr) duduk bersama kepala sekolah (pr) ?</t>
+  </si>
+  <si>
+    <t>dimana rumah kepala sekolah (pr) ?</t>
+  </si>
+  <si>
+    <t>dimana suadu (pr) meletakkan sapu (tsb) ?</t>
   </si>
 </sst>
 </file>
@@ -461,18 +599,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB1D26F8-1865-41B3-B896-C0550BDC1135}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E14"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48:A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="76" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="76" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -486,10 +624,13 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -502,11 +643,11 @@
       <c r="D2">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -519,11 +660,11 @@
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -536,11 +677,11 @@
       <c r="D4">
         <v>0</v>
       </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -553,11 +694,11 @@
       <c r="D5">
         <v>0</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -570,11 +711,11 @@
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -587,11 +728,11 @@
       <c r="D7">
         <v>0</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -604,11 +745,11 @@
       <c r="D8">
         <v>0</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -621,11 +762,11 @@
       <c r="D9">
         <v>0</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -638,11 +779,11 @@
       <c r="D10">
         <v>0</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -655,11 +796,11 @@
       <c r="D11">
         <v>0</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -672,11 +813,11 @@
       <c r="D12">
         <v>0</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -689,11 +830,11 @@
       <c r="D13">
         <v>0</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -706,8 +847,908 @@
       <c r="D14">
         <v>0</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>7</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>46</v>
+      </c>
+      <c r="F15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>7</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>46</v>
+      </c>
+      <c r="F16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>7</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>46</v>
+      </c>
+      <c r="F17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>7</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>46</v>
+      </c>
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>7</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>46</v>
+      </c>
+      <c r="F19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>7</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>46</v>
+      </c>
+      <c r="F20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>7</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>46</v>
+      </c>
+      <c r="F21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>7</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>46</v>
+      </c>
+      <c r="F22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>7</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>46</v>
+      </c>
+      <c r="F23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>7</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>46</v>
+      </c>
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>7</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>46</v>
+      </c>
+      <c r="F25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>7</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>46</v>
+      </c>
+      <c r="F26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>7</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>46</v>
+      </c>
+      <c r="F27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>7</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>46</v>
+      </c>
+      <c r="F28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>7</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>47</v>
+      </c>
+      <c r="F29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>7</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>47</v>
+      </c>
+      <c r="F30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>7</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>47</v>
+      </c>
+      <c r="F31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <v>7</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>47</v>
+      </c>
+      <c r="F32" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33">
+        <v>7</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>47</v>
+      </c>
+      <c r="F33" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <v>7</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>47</v>
+      </c>
+      <c r="F34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <v>7</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>47</v>
+      </c>
+      <c r="F35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>7</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>47</v>
+      </c>
+      <c r="F36" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37">
+        <v>7</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>47</v>
+      </c>
+      <c r="F37" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38">
+        <v>7</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>47</v>
+      </c>
+      <c r="F38" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39">
+        <v>7</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>47</v>
+      </c>
+      <c r="F39" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40">
+        <v>7</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>47</v>
+      </c>
+      <c r="F40" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <v>7</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>47</v>
+      </c>
+      <c r="F41" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42">
+        <v>7</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>47</v>
+      </c>
+      <c r="F42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43">
+        <v>7</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>47</v>
+      </c>
+      <c r="F43" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44">
+        <v>7</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>48</v>
+      </c>
+      <c r="F44" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="C45">
+        <v>7</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>48</v>
+      </c>
+      <c r="F45" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+      <c r="C46">
+        <v>7</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>48</v>
+      </c>
+      <c r="F46" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47">
+        <v>7</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>48</v>
+      </c>
+      <c r="F47" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
+      </c>
+      <c r="C48">
+        <v>7</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>48</v>
+      </c>
+      <c r="F48" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>2</v>
+      </c>
+      <c r="C49">
+        <v>7</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>48</v>
+      </c>
+      <c r="F49" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>2</v>
+      </c>
+      <c r="C50">
+        <v>7</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>48</v>
+      </c>
+      <c r="F50" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>2</v>
+      </c>
+      <c r="C51">
+        <v>7</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>48</v>
+      </c>
+      <c r="F51" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52">
+        <v>7</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>48</v>
+      </c>
+      <c r="F52" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>2</v>
+      </c>
+      <c r="C53">
+        <v>7</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>48</v>
+      </c>
+      <c r="F53" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>2</v>
+      </c>
+      <c r="C54">
+        <v>7</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>48</v>
+      </c>
+      <c r="F54" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>2</v>
+      </c>
+      <c r="C55">
+        <v>7</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>48</v>
+      </c>
+      <c r="F55" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>2</v>
+      </c>
+      <c r="C56">
+        <v>7</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>48</v>
+      </c>
+      <c r="F56" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>2</v>
+      </c>
+      <c r="C57">
+        <v>7</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>48</v>
+      </c>
+      <c r="F57" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>2</v>
+      </c>
+      <c r="C58">
+        <v>7</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <v>48</v>
+      </c>
+      <c r="F58" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>2</v>
+      </c>
+      <c r="C59">
+        <v>7</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>48</v>
+      </c>
+      <c r="F59" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add juz 1 filter, 1p5-11
</commit_message>
<xml_diff>
--- a/data kalimat durusul lughoh 2.xlsx
+++ b/data kalimat durusul lughoh 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\trial\githurtfmplizio\rtfmpliz.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E91EAB4-67CE-4962-8B1E-7369165E7E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF950DE6-B71C-4D4B-AB60-BF5381115BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7410" yWindow="0" windowWidth="13185" windowHeight="10905" xr2:uid="{998D3561-EEEE-4E4F-800B-72A3D3D90E3C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{998D3561-EEEE-4E4F-800B-72A3D3D90E3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="174">
   <si>
     <t>id</t>
   </si>
@@ -423,6 +423,141 @@
   </si>
   <si>
     <t>apakah kalian (lk/pr) telah mendengar adzan (tsb) wahai saudara-sauadraku (lk/pr) ?</t>
+  </si>
+  <si>
+    <t>ini (adalah) rumah</t>
+  </si>
+  <si>
+    <t>ini  (adalah) masjid</t>
+  </si>
+  <si>
+    <t>ini  (adalah) pintu</t>
+  </si>
+  <si>
+    <t>ini  (adalah) buku</t>
+  </si>
+  <si>
+    <t>ini  (adalah) pena</t>
+  </si>
+  <si>
+    <t>ini  (adalah) kunci</t>
+  </si>
+  <si>
+    <t>ini  (adalah) meja</t>
+  </si>
+  <si>
+    <t>ini  (adalah) ranjang</t>
+  </si>
+  <si>
+    <t>ini  (adalah) kursi</t>
+  </si>
+  <si>
+    <t>apa ini</t>
+  </si>
+  <si>
+    <t>apakah ini rumah ?</t>
+  </si>
+  <si>
+    <t>ya, ini  (adalah) rumah</t>
+  </si>
+  <si>
+    <t>ini adalah baju</t>
+  </si>
+  <si>
+    <t>apakah ini ranjang ?</t>
+  </si>
+  <si>
+    <t>tidak, ini  (adalah) kursi</t>
+  </si>
+  <si>
+    <t>apakah ini kunci</t>
+  </si>
+  <si>
+    <t>tidak , ini  (adalah) pena</t>
+  </si>
+  <si>
+    <t>ini  (adalah) bintang</t>
+  </si>
+  <si>
+    <t>siapa ini ?</t>
+  </si>
+  <si>
+    <t>ini  (adalah) dokter</t>
+  </si>
+  <si>
+    <t>ini  (adalah) murid</t>
+  </si>
+  <si>
+    <t>ini  (adalah) anak laki-laki</t>
+  </si>
+  <si>
+    <t>ini  (adalah) laki-laki</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (adalah)</t>
+  </si>
+  <si>
+    <t>ini  (adalah) anjing</t>
+  </si>
+  <si>
+    <t>ini  (adalah) keledai</t>
+  </si>
+  <si>
+    <t>tidak, ini  (adalah) kucing</t>
+  </si>
+  <si>
+    <t>ini  (adalah) pedagang</t>
+  </si>
+  <si>
+    <t>apakah ini keledai ?</t>
+  </si>
+  <si>
+    <t>apakah ini anjing ?</t>
+  </si>
+  <si>
+    <t>tidak, ini  (adalah) kuda</t>
+  </si>
+  <si>
+    <t>dan apa ini ?</t>
+  </si>
+  <si>
+    <t>ini  (adalah) unta</t>
+  </si>
+  <si>
+    <t>ini  (adalah) ayam jago</t>
+  </si>
+  <si>
+    <t>ini  (adalah) guru</t>
+  </si>
+  <si>
+    <t>apakah ini baju ?</t>
+  </si>
+  <si>
+    <t>tidak, ini  (adalah) serbet</t>
+  </si>
+  <si>
+    <t>apa ini &gt; ini  (adalah) pena</t>
+  </si>
+  <si>
+    <t>siapa ini ? Ini  (adalah) dokter</t>
+  </si>
+  <si>
+    <t>apakah ini anjing ? Tidak, ini  (adalah) kucing</t>
+  </si>
+  <si>
+    <t>apakah ini ayam jago ? Ya</t>
+  </si>
+  <si>
+    <t>apakah ini kuda ? Tidak ini  (adalah) keledai</t>
+  </si>
+  <si>
+    <t>apakah ini anak laki-laki ? Ya</t>
+  </si>
+  <si>
+    <t>siapa ini ? Ini adalah laki-laki</t>
+  </si>
+  <si>
+    <t>apa itu ? Itu  (adalah) bintang</t>
   </si>
 </sst>
 </file>
@@ -801,10 +936,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB1D26F8-1865-41B3-B896-C0550BDC1135}">
-  <dimension ref="A1:F124"/>
+  <dimension ref="A1:G168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection sqref="A1:F124"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="69" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G160" sqref="G160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2192,7 +2328,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -2212,7 +2348,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2232,7 +2368,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2252,7 +2388,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2272,7 +2408,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2292,7 +2428,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2312,7 +2448,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2332,7 +2468,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2352,7 +2488,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2372,7 +2508,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2392,7 +2528,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2412,7 +2548,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2432,7 +2568,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2452,7 +2588,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2472,7 +2608,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2492,7 +2628,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2512,7 +2648,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2532,7 +2668,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2552,7 +2688,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2572,7 +2708,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2592,7 +2728,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2612,7 +2748,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2632,7 +2768,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2652,7 +2788,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2672,7 +2808,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -2692,7 +2828,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -2712,7 +2848,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -2732,7 +2868,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -2752,7 +2888,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -2772,7 +2908,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -2792,7 +2928,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -2812,7 +2948,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -2832,7 +2968,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -2852,7 +2988,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -2872,7 +3008,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -2892,7 +3028,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -2912,7 +3048,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -2932,7 +3068,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -2952,7 +3088,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -2972,7 +3108,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -2992,7 +3128,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -3012,7 +3148,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -3032,7 +3168,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -3052,7 +3188,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -3072,7 +3208,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -3092,7 +3228,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -3112,7 +3248,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -3132,7 +3268,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -3152,7 +3288,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -3172,7 +3308,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -3192,7 +3328,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -3212,7 +3348,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
@@ -3232,7 +3368,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
@@ -3252,7 +3388,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
@@ -3272,7 +3408,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
@@ -3290,6 +3426,883 @@
       </c>
       <c r="F124" t="s">
         <v>127</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>124</v>
+      </c>
+      <c r="B125">
+        <v>1</v>
+      </c>
+      <c r="C125">
+        <v>1</v>
+      </c>
+      <c r="D125">
+        <v>0</v>
+      </c>
+      <c r="E125">
+        <v>5</v>
+      </c>
+      <c r="F125" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>125</v>
+      </c>
+      <c r="B126">
+        <v>1</v>
+      </c>
+      <c r="C126">
+        <v>1</v>
+      </c>
+      <c r="D126">
+        <v>0</v>
+      </c>
+      <c r="E126">
+        <v>5</v>
+      </c>
+      <c r="F126" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>126</v>
+      </c>
+      <c r="B127">
+        <v>1</v>
+      </c>
+      <c r="C127">
+        <v>1</v>
+      </c>
+      <c r="D127">
+        <v>0</v>
+      </c>
+      <c r="E127">
+        <v>5</v>
+      </c>
+      <c r="F127" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>127</v>
+      </c>
+      <c r="B128">
+        <v>1</v>
+      </c>
+      <c r="C128">
+        <v>1</v>
+      </c>
+      <c r="D128">
+        <v>0</v>
+      </c>
+      <c r="E128">
+        <v>5</v>
+      </c>
+      <c r="F128" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>128</v>
+      </c>
+      <c r="B129">
+        <v>1</v>
+      </c>
+      <c r="C129">
+        <v>1</v>
+      </c>
+      <c r="D129">
+        <v>0</v>
+      </c>
+      <c r="E129">
+        <v>5</v>
+      </c>
+      <c r="F129" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>129</v>
+      </c>
+      <c r="B130">
+        <v>1</v>
+      </c>
+      <c r="C130">
+        <v>1</v>
+      </c>
+      <c r="D130">
+        <v>0</v>
+      </c>
+      <c r="E130">
+        <v>5</v>
+      </c>
+      <c r="F130" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>130</v>
+      </c>
+      <c r="B131">
+        <v>1</v>
+      </c>
+      <c r="C131">
+        <v>1</v>
+      </c>
+      <c r="D131">
+        <v>0</v>
+      </c>
+      <c r="E131">
+        <v>5</v>
+      </c>
+      <c r="F131" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>131</v>
+      </c>
+      <c r="B132">
+        <v>1</v>
+      </c>
+      <c r="C132">
+        <v>1</v>
+      </c>
+      <c r="D132">
+        <v>0</v>
+      </c>
+      <c r="E132">
+        <v>5</v>
+      </c>
+      <c r="F132" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>132</v>
+      </c>
+      <c r="B133">
+        <v>1</v>
+      </c>
+      <c r="C133">
+        <v>1</v>
+      </c>
+      <c r="D133">
+        <v>0</v>
+      </c>
+      <c r="E133">
+        <v>5</v>
+      </c>
+      <c r="F133" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>133</v>
+      </c>
+      <c r="B134">
+        <v>1</v>
+      </c>
+      <c r="C134">
+        <v>1</v>
+      </c>
+      <c r="D134">
+        <v>0</v>
+      </c>
+      <c r="E134">
+        <v>6</v>
+      </c>
+      <c r="F134" t="s">
+        <v>138</v>
+      </c>
+      <c r="G134" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>134</v>
+      </c>
+      <c r="B135">
+        <v>1</v>
+      </c>
+      <c r="C135">
+        <v>1</v>
+      </c>
+      <c r="D135">
+        <v>0</v>
+      </c>
+      <c r="E135">
+        <v>6</v>
+      </c>
+      <c r="F135" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>135</v>
+      </c>
+      <c r="B136">
+        <v>1</v>
+      </c>
+      <c r="C136">
+        <v>1</v>
+      </c>
+      <c r="D136">
+        <v>0</v>
+      </c>
+      <c r="E136">
+        <v>6</v>
+      </c>
+      <c r="F136" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>136</v>
+      </c>
+      <c r="B137">
+        <v>1</v>
+      </c>
+      <c r="C137">
+        <v>1</v>
+      </c>
+      <c r="D137">
+        <v>0</v>
+      </c>
+      <c r="E137">
+        <v>6</v>
+      </c>
+      <c r="F137" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>137</v>
+      </c>
+      <c r="B138">
+        <v>1</v>
+      </c>
+      <c r="C138">
+        <v>1</v>
+      </c>
+      <c r="D138">
+        <v>0</v>
+      </c>
+      <c r="E138">
+        <v>6</v>
+      </c>
+      <c r="F138" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>138</v>
+      </c>
+      <c r="B139">
+        <v>1</v>
+      </c>
+      <c r="C139">
+        <v>1</v>
+      </c>
+      <c r="D139">
+        <v>0</v>
+      </c>
+      <c r="E139">
+        <v>6</v>
+      </c>
+      <c r="F139" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>139</v>
+      </c>
+      <c r="B140">
+        <v>1</v>
+      </c>
+      <c r="C140">
+        <v>1</v>
+      </c>
+      <c r="D140">
+        <v>0</v>
+      </c>
+      <c r="E140">
+        <v>6</v>
+      </c>
+      <c r="F140" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>140</v>
+      </c>
+      <c r="B141">
+        <v>1</v>
+      </c>
+      <c r="C141">
+        <v>1</v>
+      </c>
+      <c r="D141">
+        <v>0</v>
+      </c>
+      <c r="E141">
+        <v>6</v>
+      </c>
+      <c r="F141" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>141</v>
+      </c>
+      <c r="B142">
+        <v>1</v>
+      </c>
+      <c r="C142">
+        <v>1</v>
+      </c>
+      <c r="D142">
+        <v>0</v>
+      </c>
+      <c r="E142">
+        <v>6</v>
+      </c>
+      <c r="F142" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>142</v>
+      </c>
+      <c r="B143">
+        <v>1</v>
+      </c>
+      <c r="C143">
+        <v>1</v>
+      </c>
+      <c r="D143">
+        <v>0</v>
+      </c>
+      <c r="E143">
+        <v>9</v>
+      </c>
+      <c r="F143" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>143</v>
+      </c>
+      <c r="B144">
+        <v>1</v>
+      </c>
+      <c r="C144">
+        <v>1</v>
+      </c>
+      <c r="D144">
+        <v>0</v>
+      </c>
+      <c r="E144">
+        <v>9</v>
+      </c>
+      <c r="F144" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>144</v>
+      </c>
+      <c r="B145">
+        <v>1</v>
+      </c>
+      <c r="C145">
+        <v>1</v>
+      </c>
+      <c r="D145">
+        <v>0</v>
+      </c>
+      <c r="E145">
+        <v>9</v>
+      </c>
+      <c r="F145" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>145</v>
+      </c>
+      <c r="B146">
+        <v>1</v>
+      </c>
+      <c r="C146">
+        <v>1</v>
+      </c>
+      <c r="D146">
+        <v>0</v>
+      </c>
+      <c r="E146">
+        <v>9</v>
+      </c>
+      <c r="F146" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>146</v>
+      </c>
+      <c r="B147">
+        <v>1</v>
+      </c>
+      <c r="C147">
+        <v>1</v>
+      </c>
+      <c r="D147">
+        <v>0</v>
+      </c>
+      <c r="E147">
+        <v>9</v>
+      </c>
+      <c r="F147" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>147</v>
+      </c>
+      <c r="B148">
+        <v>1</v>
+      </c>
+      <c r="C148">
+        <v>1</v>
+      </c>
+      <c r="D148">
+        <v>0</v>
+      </c>
+      <c r="E148">
+        <v>10</v>
+      </c>
+      <c r="F148" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>148</v>
+      </c>
+      <c r="B149">
+        <v>1</v>
+      </c>
+      <c r="C149">
+        <v>1</v>
+      </c>
+      <c r="D149">
+        <v>0</v>
+      </c>
+      <c r="E149">
+        <v>10</v>
+      </c>
+      <c r="F149" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>149</v>
+      </c>
+      <c r="B150">
+        <v>1</v>
+      </c>
+      <c r="C150">
+        <v>1</v>
+      </c>
+      <c r="D150">
+        <v>0</v>
+      </c>
+      <c r="E150">
+        <v>10</v>
+      </c>
+      <c r="F150" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>150</v>
+      </c>
+      <c r="B151">
+        <v>1</v>
+      </c>
+      <c r="C151">
+        <v>1</v>
+      </c>
+      <c r="D151">
+        <v>0</v>
+      </c>
+      <c r="E151">
+        <v>10</v>
+      </c>
+      <c r="F151" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>151</v>
+      </c>
+      <c r="B152">
+        <v>1</v>
+      </c>
+      <c r="C152">
+        <v>1</v>
+      </c>
+      <c r="D152">
+        <v>0</v>
+      </c>
+      <c r="E152">
+        <v>10</v>
+      </c>
+      <c r="F152" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>152</v>
+      </c>
+      <c r="B153">
+        <v>1</v>
+      </c>
+      <c r="C153">
+        <v>1</v>
+      </c>
+      <c r="D153">
+        <v>0</v>
+      </c>
+      <c r="E153">
+        <v>10</v>
+      </c>
+      <c r="F153" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>153</v>
+      </c>
+      <c r="B154">
+        <v>1</v>
+      </c>
+      <c r="C154">
+        <v>1</v>
+      </c>
+      <c r="D154">
+        <v>0</v>
+      </c>
+      <c r="E154">
+        <v>10</v>
+      </c>
+      <c r="F154" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>154</v>
+      </c>
+      <c r="B155">
+        <v>1</v>
+      </c>
+      <c r="C155">
+        <v>1</v>
+      </c>
+      <c r="D155">
+        <v>0</v>
+      </c>
+      <c r="E155">
+        <v>10</v>
+      </c>
+      <c r="F155" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>155</v>
+      </c>
+      <c r="B156">
+        <v>1</v>
+      </c>
+      <c r="C156">
+        <v>1</v>
+      </c>
+      <c r="D156">
+        <v>0</v>
+      </c>
+      <c r="E156">
+        <v>10</v>
+      </c>
+      <c r="F156" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>156</v>
+      </c>
+      <c r="B157">
+        <v>1</v>
+      </c>
+      <c r="C157">
+        <v>1</v>
+      </c>
+      <c r="D157">
+        <v>0</v>
+      </c>
+      <c r="E157">
+        <v>11</v>
+      </c>
+      <c r="F157" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>157</v>
+      </c>
+      <c r="B158">
+        <v>1</v>
+      </c>
+      <c r="C158">
+        <v>1</v>
+      </c>
+      <c r="D158">
+        <v>0</v>
+      </c>
+      <c r="E158">
+        <v>11</v>
+      </c>
+      <c r="F158" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>158</v>
+      </c>
+      <c r="B159">
+        <v>1</v>
+      </c>
+      <c r="C159">
+        <v>1</v>
+      </c>
+      <c r="D159">
+        <v>0</v>
+      </c>
+      <c r="E159">
+        <v>11</v>
+      </c>
+      <c r="F159" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>159</v>
+      </c>
+      <c r="B160">
+        <v>1</v>
+      </c>
+      <c r="C160">
+        <v>1</v>
+      </c>
+      <c r="D160">
+        <v>0</v>
+      </c>
+      <c r="E160">
+        <v>11</v>
+      </c>
+      <c r="F160" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>160</v>
+      </c>
+      <c r="B161">
+        <v>1</v>
+      </c>
+      <c r="C161">
+        <v>1</v>
+      </c>
+      <c r="D161">
+        <v>0</v>
+      </c>
+      <c r="E161">
+        <v>11</v>
+      </c>
+      <c r="F161" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>161</v>
+      </c>
+      <c r="B162">
+        <v>1</v>
+      </c>
+      <c r="C162">
+        <v>1</v>
+      </c>
+      <c r="D162">
+        <v>0</v>
+      </c>
+      <c r="E162">
+        <v>11</v>
+      </c>
+      <c r="F162" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>162</v>
+      </c>
+      <c r="B163">
+        <v>1</v>
+      </c>
+      <c r="C163">
+        <v>1</v>
+      </c>
+      <c r="D163">
+        <v>0</v>
+      </c>
+      <c r="E163">
+        <v>11</v>
+      </c>
+      <c r="F163" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>163</v>
+      </c>
+      <c r="B164">
+        <v>1</v>
+      </c>
+      <c r="C164">
+        <v>1</v>
+      </c>
+      <c r="D164">
+        <v>0</v>
+      </c>
+      <c r="E164">
+        <v>11</v>
+      </c>
+      <c r="F164" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>164</v>
+      </c>
+      <c r="B165">
+        <v>1</v>
+      </c>
+      <c r="C165">
+        <v>1</v>
+      </c>
+      <c r="D165">
+        <v>0</v>
+      </c>
+      <c r="E165">
+        <v>11</v>
+      </c>
+      <c r="F165" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>165</v>
+      </c>
+      <c r="B166">
+        <v>1</v>
+      </c>
+      <c r="C166">
+        <v>1</v>
+      </c>
+      <c r="D166">
+        <v>0</v>
+      </c>
+      <c r="E166">
+        <v>11</v>
+      </c>
+      <c r="F166" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>166</v>
+      </c>
+      <c r="B167">
+        <v>1</v>
+      </c>
+      <c r="C167">
+        <v>1</v>
+      </c>
+      <c r="D167">
+        <v>0</v>
+      </c>
+      <c r="E167">
+        <v>11</v>
+      </c>
+      <c r="F167" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>167</v>
+      </c>
+      <c r="C168">
+        <v>2</v>
+      </c>
+      <c r="E168">
+        <v>11</v>
+      </c>
+      <c r="F168" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add dars from after add 1p5-6
</commit_message>
<xml_diff>
--- a/data kalimat durusul lughoh 2.xlsx
+++ b/data kalimat durusul lughoh 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\trial\githurtfmplizio\rtfmpliz.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF950DE6-B71C-4D4B-AB60-BF5381115BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{155DBA7D-C733-4768-A63D-09DAAC4872F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{998D3561-EEEE-4E4F-800B-72A3D3D90E3C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="193">
   <si>
     <t>id</t>
   </si>
@@ -558,6 +558,63 @@
   </si>
   <si>
     <t>apa itu ? Itu  (adalah) bintang</t>
+  </si>
+  <si>
+    <t>bagaimana kabarmu wahai Ustadz ? Semoga kamu dalam keadaan baik</t>
+  </si>
+  <si>
+    <t>alhamdulillah, dan bagaimana kabarmu wahai hasyim, ? Saya mencintaimu dengan banyak wahai hasyim, sesungguhnya engkau adalah murid yang pandai dan rajin dan memiliki akhlaq yang baik. Apakah dari pakistan kamu atau dari india wahai hasyim ?</t>
+  </si>
+  <si>
+    <t>sesungguhnya aku dari india</t>
+  </si>
+  <si>
+    <t>dan temanku yang keluar bersamamu sekarang dari kelas, apakah dia juga dari india ?</t>
+  </si>
+  <si>
+    <t>tidak, sesungguhnya dia dari pakistan</t>
+  </si>
+  <si>
+    <t>sesungguhnya jam tangan mu indah wahai hasyim, apakah dari jepang dia (jam) ?</t>
+  </si>
+  <si>
+    <t>tidak, sesungguhnya dia (jam) dari india</t>
+  </si>
+  <si>
+    <t>apakah dia (jam) mahal atau murah ?</t>
+  </si>
+  <si>
+    <t>sesungguhnya dia (jam) murah sekali. Sesungguhnya dengan 100 rupiah saja</t>
+  </si>
+  <si>
+    <t>berapa saudara laki laki (milik) mu wahai hasyim ?</t>
+  </si>
+  <si>
+    <t>aku memiliki 3 saudara laki-laki</t>
+  </si>
+  <si>
+    <t>apakah murid-murid (mereka) ?</t>
+  </si>
+  <si>
+    <t>tida sesungguhnya mereka (lk) (adalah) para pedagang</t>
+  </si>
+  <si>
+    <t>dan berapa saudara (pr) milikmu ?</t>
+  </si>
+  <si>
+    <t>aku memiliki 4 saudara (pr)</t>
+  </si>
+  <si>
+    <t>apakah di india mereka (pr) sekarang ?</t>
+  </si>
+  <si>
+    <t>tidak, sesungguhnya mereka (pr) dengan (di) madinah munawaroh bersama bapakku dan ibuku</t>
+  </si>
+  <si>
+    <t>apakah murid-murid (mereka pr) ?</t>
+  </si>
+  <si>
+    <t>tidak, sesungguhnya mereka (pr) adalah guru-guru (pr) madrasah tsanawiyah</t>
   </si>
 </sst>
 </file>
@@ -936,11 +993,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB1D26F8-1865-41B3-B896-C0550BDC1135}">
-  <dimension ref="A1:G168"/>
+  <dimension ref="A1:G187"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="69" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G160" sqref="G160"/>
+      <pane ySplit="1" topLeftCell="A177" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A167" sqref="A167:A187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,7 +1025,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -988,7 +1045,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1008,7 +1065,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1028,7 +1085,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1048,7 +1105,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1068,7 +1125,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1088,7 +1145,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1108,7 +1165,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1128,7 +1185,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1148,7 +1205,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1168,7 +1225,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1188,7 +1245,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1208,7 +1265,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1228,7 +1285,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1248,7 +1305,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1268,7 +1325,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1288,7 +1345,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1308,7 +1365,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1328,7 +1385,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1348,7 +1405,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1368,7 +1425,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1388,7 +1445,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1408,7 +1465,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1428,7 +1485,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1448,7 +1505,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1468,7 +1525,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1488,7 +1545,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1508,7 +1565,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1528,7 +1585,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1548,7 +1605,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1568,7 +1625,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1588,7 +1645,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1608,7 +1665,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1628,7 +1685,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1648,7 +1705,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1668,7 +1725,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1688,7 +1745,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1708,7 +1765,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1728,7 +1785,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1748,7 +1805,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1768,7 +1825,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1788,7 +1845,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1808,7 +1865,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1828,7 +1885,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1848,7 +1905,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1868,7 +1925,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1888,7 +1945,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1908,7 +1965,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1928,7 +1985,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1948,7 +2005,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1968,7 +2025,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1988,7 +2045,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2008,7 +2065,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2028,7 +2085,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2048,7 +2105,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2068,7 +2125,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2088,7 +2145,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2108,7 +2165,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2128,7 +2185,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2148,7 +2205,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2168,7 +2225,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2188,7 +2245,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2208,7 +2265,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2228,7 +2285,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2248,7 +2305,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2268,7 +2325,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2288,7 +2345,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2308,7 +2365,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2328,7 +2385,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -2348,7 +2405,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2368,7 +2425,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2388,7 +2445,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2408,7 +2465,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2428,7 +2485,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2448,7 +2505,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2468,7 +2525,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2488,7 +2545,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2508,7 +2565,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2528,7 +2585,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2548,7 +2605,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2568,7 +2625,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2588,7 +2645,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2608,7 +2665,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2628,7 +2685,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2648,7 +2705,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2668,7 +2725,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2688,7 +2745,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2708,7 +2765,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2728,7 +2785,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2748,7 +2805,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2768,7 +2825,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2788,7 +2845,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2808,7 +2865,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -2828,7 +2885,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -2848,7 +2905,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -2868,7 +2925,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -2888,7 +2945,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -2908,7 +2965,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -2928,7 +2985,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -2948,7 +3005,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -2968,7 +3025,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -2988,7 +3045,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -3008,7 +3065,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -3028,7 +3085,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -3048,7 +3105,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -3068,7 +3125,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -3088,7 +3145,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -3108,7 +3165,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -3128,7 +3185,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -3148,7 +3205,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -3168,7 +3225,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -3188,7 +3245,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -3208,7 +3265,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -3228,7 +3285,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -3248,7 +3305,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -3268,7 +3325,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -3288,7 +3345,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -3308,7 +3365,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -3328,7 +3385,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -3348,7 +3405,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
@@ -3368,7 +3425,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
@@ -3388,7 +3445,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
@@ -3408,7 +3465,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
@@ -4295,14 +4352,400 @@
       <c r="A168">
         <v>167</v>
       </c>
+      <c r="B168">
+        <v>1</v>
+      </c>
       <c r="C168">
         <v>2</v>
+      </c>
+      <c r="D168">
+        <v>0</v>
       </c>
       <c r="E168">
         <v>11</v>
       </c>
       <c r="F168" t="s">
         <v>173</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>168</v>
+      </c>
+      <c r="B169">
+        <v>2</v>
+      </c>
+      <c r="C169">
+        <v>1</v>
+      </c>
+      <c r="D169">
+        <v>0</v>
+      </c>
+      <c r="E169">
+        <v>5</v>
+      </c>
+      <c r="F169" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>169</v>
+      </c>
+      <c r="B170">
+        <v>2</v>
+      </c>
+      <c r="C170">
+        <v>1</v>
+      </c>
+      <c r="D170">
+        <v>0</v>
+      </c>
+      <c r="E170">
+        <v>5</v>
+      </c>
+      <c r="F170" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>170</v>
+      </c>
+      <c r="B171">
+        <v>2</v>
+      </c>
+      <c r="C171">
+        <v>1</v>
+      </c>
+      <c r="D171">
+        <v>0</v>
+      </c>
+      <c r="E171">
+        <v>5</v>
+      </c>
+      <c r="F171" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>171</v>
+      </c>
+      <c r="B172">
+        <v>2</v>
+      </c>
+      <c r="C172">
+        <v>1</v>
+      </c>
+      <c r="D172">
+        <v>0</v>
+      </c>
+      <c r="E172">
+        <v>5</v>
+      </c>
+      <c r="F172" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>172</v>
+      </c>
+      <c r="B173">
+        <v>2</v>
+      </c>
+      <c r="C173">
+        <v>1</v>
+      </c>
+      <c r="D173">
+        <v>0</v>
+      </c>
+      <c r="E173">
+        <v>5</v>
+      </c>
+      <c r="F173" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>173</v>
+      </c>
+      <c r="B174">
+        <v>2</v>
+      </c>
+      <c r="C174">
+        <v>1</v>
+      </c>
+      <c r="D174">
+        <v>0</v>
+      </c>
+      <c r="E174">
+        <v>5</v>
+      </c>
+      <c r="F174" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>174</v>
+      </c>
+      <c r="B175">
+        <v>2</v>
+      </c>
+      <c r="C175">
+        <v>1</v>
+      </c>
+      <c r="D175">
+        <v>0</v>
+      </c>
+      <c r="E175">
+        <v>5</v>
+      </c>
+      <c r="F175" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>175</v>
+      </c>
+      <c r="B176">
+        <v>2</v>
+      </c>
+      <c r="C176">
+        <v>1</v>
+      </c>
+      <c r="D176">
+        <v>0</v>
+      </c>
+      <c r="E176">
+        <v>5</v>
+      </c>
+      <c r="F176" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>176</v>
+      </c>
+      <c r="B177">
+        <v>2</v>
+      </c>
+      <c r="C177">
+        <v>1</v>
+      </c>
+      <c r="D177">
+        <v>0</v>
+      </c>
+      <c r="E177">
+        <v>5</v>
+      </c>
+      <c r="F177" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>177</v>
+      </c>
+      <c r="B178">
+        <v>2</v>
+      </c>
+      <c r="C178">
+        <v>1</v>
+      </c>
+      <c r="D178">
+        <v>0</v>
+      </c>
+      <c r="E178">
+        <v>5</v>
+      </c>
+      <c r="F178" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>178</v>
+      </c>
+      <c r="B179">
+        <v>2</v>
+      </c>
+      <c r="C179">
+        <v>1</v>
+      </c>
+      <c r="D179">
+        <v>0</v>
+      </c>
+      <c r="E179">
+        <v>6</v>
+      </c>
+      <c r="F179" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>179</v>
+      </c>
+      <c r="B180">
+        <v>2</v>
+      </c>
+      <c r="C180">
+        <v>1</v>
+      </c>
+      <c r="D180">
+        <v>0</v>
+      </c>
+      <c r="E180">
+        <v>6</v>
+      </c>
+      <c r="F180" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>180</v>
+      </c>
+      <c r="B181">
+        <v>2</v>
+      </c>
+      <c r="C181">
+        <v>1</v>
+      </c>
+      <c r="D181">
+        <v>0</v>
+      </c>
+      <c r="E181">
+        <v>6</v>
+      </c>
+      <c r="F181" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>181</v>
+      </c>
+      <c r="B182">
+        <v>2</v>
+      </c>
+      <c r="C182">
+        <v>1</v>
+      </c>
+      <c r="D182">
+        <v>0</v>
+      </c>
+      <c r="E182">
+        <v>6</v>
+      </c>
+      <c r="F182" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>182</v>
+      </c>
+      <c r="B183">
+        <v>2</v>
+      </c>
+      <c r="C183">
+        <v>1</v>
+      </c>
+      <c r="D183">
+        <v>0</v>
+      </c>
+      <c r="E183">
+        <v>6</v>
+      </c>
+      <c r="F183" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>183</v>
+      </c>
+      <c r="B184">
+        <v>2</v>
+      </c>
+      <c r="C184">
+        <v>1</v>
+      </c>
+      <c r="D184">
+        <v>0</v>
+      </c>
+      <c r="E184">
+        <v>6</v>
+      </c>
+      <c r="F184" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>184</v>
+      </c>
+      <c r="B185">
+        <v>2</v>
+      </c>
+      <c r="C185">
+        <v>1</v>
+      </c>
+      <c r="D185">
+        <v>0</v>
+      </c>
+      <c r="E185">
+        <v>6</v>
+      </c>
+      <c r="F185" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>185</v>
+      </c>
+      <c r="B186">
+        <v>2</v>
+      </c>
+      <c r="C186">
+        <v>1</v>
+      </c>
+      <c r="D186">
+        <v>0</v>
+      </c>
+      <c r="E186">
+        <v>6</v>
+      </c>
+      <c r="F186" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>186</v>
+      </c>
+      <c r="B187">
+        <v>2</v>
+      </c>
+      <c r="C187">
+        <v>1</v>
+      </c>
+      <c r="D187">
+        <v>0</v>
+      </c>
+      <c r="E187">
+        <v>6</v>
+      </c>
+      <c r="F187" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>